<commit_message>
yield prediction files from rtRBA
</commit_message>
<xml_diff>
--- a/application/cerevisiae_compiled_results.xlsx
+++ b/application/cerevisiae_compiled_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/rtRBA-main/application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0172825C-B5BB-6547-B0F0-4E0488C00C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF0097-C55D-5F42-B04F-0D88C41394CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="760" windowWidth="16260" windowHeight="17580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="from github" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'from github'!$D$2:$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -974,7 +973,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:Q30"/>
+      <selection pane="bottomLeft" activeCell="Q30" sqref="A1:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2682,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C57BD-CD57-BA47-A7EF-9AFB3CBA4A3F}">
   <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>